<commit_message>
Small update to Excel Data
</commit_message>
<xml_diff>
--- a/DevDeck Experiment Graph.xlsx
+++ b/DevDeck Experiment Graph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanc\UML\COMP 4120\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ryanc\Comp4120\DevDeck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9B51F6-66C3-4DCC-8AB7-87CF31FC52AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0FA1DF-6277-4D34-833A-AFC601E5A0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EBFF282B-049A-4F1B-97A5-54CBB5C1F0C2}"/>
   </bookViews>
@@ -305,7 +305,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1297,12 +1297,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A8717578-0C13-4604-BE8E-BDE85625561D}" name="Table1" displayName="Table1" ref="E5:G9" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A8717578-0C13-4604-BE8E-BDE85625561D}" name="Table1" displayName="Table1" ref="E5:G9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="E5:G9" xr:uid="{A8717578-0C13-4604-BE8E-BDE85625561D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{B832A243-DC04-4224-9A7C-20AB0A2B8DC0}" name="Name" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{976563BB-C7F7-4506-A4DC-2FC0668CB77C}" name="First Resume Interviews" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{6C61FC03-D6DE-4024-840C-3B7BC5BB523F}" name="DevDeck Resume Interviews" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{B832A243-DC04-4224-9A7C-20AB0A2B8DC0}" name="Name" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{976563BB-C7F7-4506-A4DC-2FC0668CB77C}" name="First Resume Interviews" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{6C61FC03-D6DE-4024-840C-3B7BC5BB523F}" name="DevDeck Resume Interviews" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1628,7 +1628,7 @@
   <dimension ref="E5:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1665,7 +1665,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>

</xml_diff>